<commit_message>
core dog, kick core watdog when reflashing after system down.
Signed-off-by: daoweifan <daowei.fan@delphi.com>
</commit_message>
<xml_diff>
--- a/document/MT22P3_LLD.xlsx
+++ b/document/MT22P3_LLD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>TCR[WPEXT]||TCR[WP]</t>
   </si>
@@ -118,6 +118,30 @@
   </si>
   <si>
     <t>104.8576</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>2^24</t>
+  </si>
+  <si>
+    <t>2^25</t>
+  </si>
+  <si>
+    <t>2^24/80</t>
+  </si>
+  <si>
+    <t>2^25/80</t>
+  </si>
+  <si>
+    <t>209.7152</t>
+  </si>
+  <si>
+    <t>419.4304</t>
   </si>
 </sst>
 </file>
@@ -172,8 +196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:E11" totalsRowShown="0">
-  <autoFilter ref="B2:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:E13" totalsRowShown="0">
+  <autoFilter ref="B2:E13"/>
   <tableColumns count="4">
     <tableColumn id="1" name="TCR[WPEXT]||TCR[WP]"/>
     <tableColumn id="2" name="Expire Value"/>
@@ -471,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +640,34 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>